<commit_message>
cleanup: exluindo arquivos desnecessários
</commit_message>
<xml_diff>
--- a/arquivos_gerados/Banco_de_dados_GERAL_Gerado.xlsx
+++ b/arquivos_gerados/Banco_de_dados_GERAL_Gerado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LARISSA</t>
+          <t>VITÓRIA AGUILAR DA R</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,31 +492,31 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>1968.64963935</v>
+        <v>1724.4258225375</v>
       </c>
       <c r="E2" t="n">
-        <v>23.5248705</v>
+        <v>24.501578625</v>
       </c>
       <c r="F2" t="n">
-        <v>2034.5976096</v>
+        <v>1825.91572935</v>
       </c>
       <c r="G2" t="n">
-        <v>24.611328</v>
+        <v>26.1735705</v>
       </c>
       <c r="H2" t="n">
-        <v>2313.2761656</v>
+        <v>2031.6272478375</v>
       </c>
       <c r="I2" t="n">
-        <v>29.202408</v>
+        <v>29.562557625</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ELAINE</t>
+          <t>ISABELLA ALONSO NAZO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -525,31 +525,31 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>2191.3268184</v>
+        <v>2311.20892215</v>
       </c>
       <c r="E3" t="n">
-        <v>31.148712</v>
+        <v>24.3920745</v>
       </c>
       <c r="F3" t="n">
-        <v>2495.2606185375</v>
+        <v>2194.1103366</v>
       </c>
       <c r="G3" t="n">
-        <v>36.155858625</v>
+        <v>22.462938</v>
       </c>
       <c r="H3" t="n">
-        <v>2618.18733735</v>
+        <v>2481.8474343375</v>
       </c>
       <c r="I3" t="n">
-        <v>38.1810105</v>
+        <v>27.203252625</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LARISSA</t>
+          <t>MARIA FERNANDA FARIA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -558,58 +558,1708 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>1702.59727815</v>
+        <v>1927.6998450375</v>
       </c>
       <c r="E4" t="n">
-        <v>23.0971545</v>
+        <v>25.163753625</v>
       </c>
       <c r="F4" t="n">
-        <v>1774.5669084375</v>
+        <v>1776.53310375</v>
       </c>
       <c r="G4" t="n">
-        <v>24.282815625</v>
+        <v>22.6733625</v>
       </c>
       <c r="H4" t="n">
-        <v>2001.28352535</v>
+        <v>1988.99572935</v>
       </c>
       <c r="I4" t="n">
-        <v>28.0178505</v>
+        <v>26.1735705</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>KELTO</t>
+          <t>EMILLY VITORIA MARIN</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>3029.8395975375</v>
+        <v>1388.1039045375</v>
       </c>
       <c r="E5" t="n">
+        <v>22.990838625</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1446.72018735</v>
+      </c>
+      <c r="G5" t="n">
+        <v>23.9565105</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1595.0807904</v>
+      </c>
+      <c r="I5" t="n">
+        <v>26.400672</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>VITORIA DE LIMA FALC</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>13</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2466.2165016</v>
+      </c>
+      <c r="E6" t="n">
+        <v>27.318888</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2459.1974343375</v>
+      </c>
+      <c r="G6" t="n">
+        <v>27.203252625</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2661.3584808375</v>
+      </c>
+      <c r="I6" t="n">
+        <v>30.533747625</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BRENDA ZAURIZIO CHAV</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1971.34751415</v>
+      </c>
+      <c r="E7" t="n">
+        <v>18.2706345</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2047.3067733375</v>
+      </c>
+      <c r="G7" t="n">
+        <v>19.522022625</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2323.0675410375</v>
+      </c>
+      <c r="I7" t="n">
+        <v>24.065033625</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NICOLLY VITORIA NUNE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>12</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1610.6655288375</v>
+      </c>
+      <c r="E8" t="n">
+        <v>26.060387625</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1694.0904555375</v>
+      </c>
+      <c r="G8" t="n">
+        <v>27.434768625</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2239.6573209375</v>
+      </c>
+      <c r="I8" t="n">
+        <v>36.422690625</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>GREICIELY LINHARES B</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>13</v>
+      </c>
+      <c r="D9" t="n">
+        <v>750.32443335</v>
+      </c>
+      <c r="E9" t="n">
+        <v>19.4242905</v>
+      </c>
+      <c r="F9" t="n">
+        <v>922.0571161499998</v>
+      </c>
+      <c r="G9" t="n">
+        <v>22.2534945</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1264.8451380375</v>
+      </c>
+      <c r="I9" t="n">
+        <v>27.900743625</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MARCELA SANTANA DE O</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>12</v>
+      </c>
+      <c r="D10" t="n">
+        <v>822.4950337500001</v>
+      </c>
+      <c r="E10" t="n">
+        <v>20.6132625</v>
+      </c>
+      <c r="F10" t="n">
+        <v>822.4950337500001</v>
+      </c>
+      <c r="G10" t="n">
+        <v>20.6132625</v>
+      </c>
+      <c r="H10" t="n">
+        <v>768.1661133374998</v>
+      </c>
+      <c r="I10" t="n">
+        <v>19.718222625</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LUCAS ANTUNES DO CAR</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>14</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2486.66496</v>
+      </c>
+      <c r="E11" t="n">
+        <v>28.2528</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2566.1672478375</v>
+      </c>
+      <c r="G11" t="n">
+        <v>29.562557625</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2870.4508848375</v>
+      </c>
+      <c r="I11" t="n">
+        <v>34.575467625</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PEDRO HENRIQUE DIAS </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>13</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2007.56539815</v>
+      </c>
+      <c r="E12" t="n">
+        <v>26.6287545</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2149.28654415</v>
+      </c>
+      <c r="G12" t="n">
+        <v>28.9635345</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3044.0724750375</v>
+      </c>
+      <c r="I12" t="n">
+        <v>43.704653625</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MIGUEL DOS SANTOS AR</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>13</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2632.120215</v>
+      </c>
+      <c r="E13" t="n">
+        <v>25.94745</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2715.3665016</v>
+      </c>
+      <c r="G13" t="n">
+        <v>27.318888</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3023.60999415</v>
+      </c>
+      <c r="I13" t="n">
+        <v>32.3970345</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HUDSON WILLIAN FERRE</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>14</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2231.1369459375</v>
+      </c>
+      <c r="E14" t="n">
+        <v>25.386440625</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2573.4113775375</v>
+      </c>
+      <c r="G14" t="n">
+        <v>31.025228625</v>
+      </c>
+      <c r="H14" t="n">
+        <v>2633.7917313375</v>
+      </c>
+      <c r="I14" t="n">
+        <v>32.019962625</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LUAN CARDOSO BATISTA</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>14</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2885.6254176</v>
+      </c>
+      <c r="E15" t="n">
+        <v>22.884768</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3003.79584375</v>
+      </c>
+      <c r="G15" t="n">
+        <v>24.8315625</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3305.6157360375</v>
+      </c>
+      <c r="I15" t="n">
+        <v>29.803883625</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MATHEUS ROGERIO SANT</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2324.3062656</v>
+      </c>
+      <c r="E16" t="n">
+        <v>32.145408</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2409.0486630375</v>
+      </c>
+      <c r="G16" t="n">
+        <v>33.541493625</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2740.7758854</v>
+      </c>
+      <c r="I16" t="n">
+        <v>39.006522</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PEDRO HENRIQUE PEREI</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>13</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2366.3684418375</v>
+      </c>
+      <c r="E17" t="n">
+        <v>17.613977625</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2512.0717734</v>
+      </c>
+      <c r="G17" t="n">
+        <v>20.014362</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2616.4645818375</v>
+      </c>
+      <c r="I17" t="n">
+        <v>21.734177625</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ANDREY KALEBE BORGES</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>13</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3057.61931535</v>
+      </c>
+      <c r="E18" t="n">
+        <v>21.8375505</v>
+      </c>
+      <c r="F18" t="n">
+        <v>3153.5267190375</v>
+      </c>
+      <c r="G18" t="n">
+        <v>23.417573625</v>
+      </c>
+      <c r="H18" t="n">
+        <v>3206.0469084375</v>
+      </c>
+      <c r="I18" t="n">
+        <v>24.282815625</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>HUGO ALVES DA SILVA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>14</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3245.3417313375</v>
+      </c>
+      <c r="E19" t="n">
+        <v>32.019962625</v>
+      </c>
+      <c r="F19" t="n">
+        <v>3384.6810093375</v>
+      </c>
+      <c r="G19" t="n">
+        <v>34.315502625</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3720.07035375</v>
+      </c>
+      <c r="I19" t="n">
+        <v>39.8408625</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>RICARDO RONAMIGO FIL</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>12</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1581.4140486</v>
+      </c>
+      <c r="E20" t="n">
+        <v>29.683098</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1473.2251380375</v>
+      </c>
+      <c r="G20" t="n">
+        <v>27.900743625</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1784.5948323375</v>
+      </c>
+      <c r="I20" t="n">
+        <v>33.030392625</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SAMUEL SILVA FERNAND</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>11</v>
+      </c>
+      <c r="D21" t="n">
+        <v>990.8267334375001</v>
+      </c>
+      <c r="E21" t="n">
+        <v>19.132565625</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1105.23827415</v>
+      </c>
+      <c r="G21" t="n">
+        <v>21.0174345</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1377.2178264</v>
+      </c>
+      <c r="I21" t="n">
+        <v>25.498152</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>RICHARD KAUFRAN DE S</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>13</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2249.8408848375</v>
+      </c>
+      <c r="E22" t="n">
+        <v>34.575467625</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2337.69459735</v>
+      </c>
+      <c r="G22" t="n">
+        <v>36.0228105</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2724.5992806</v>
+      </c>
+      <c r="I22" t="n">
+        <v>42.396858</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>KAIO HENRIQUE SPONTO</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>14</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1999.6539045375</v>
+      </c>
+      <c r="E23" t="n">
+        <v>22.990838625</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2071.4597814</v>
+      </c>
+      <c r="G23" t="n">
+        <v>24.173802</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2369.4389115375</v>
+      </c>
+      <c r="I23" t="n">
+        <v>29.082848625</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>GUILHERME DOS SANTOS</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>13</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1676.3436246</v>
+      </c>
+      <c r="E24" t="n">
+        <v>25.052778</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1737.5055288375</v>
+      </c>
+      <c r="G24" t="n">
+        <v>26.060387625</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2366.4973209375</v>
+      </c>
+      <c r="I24" t="n">
+        <v>36.422690625</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>GUILHERME BONFIM SAN</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>14</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2938.2626340375</v>
+      </c>
+      <c r="E25" t="n">
+        <v>20.916023625</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2987.9245818375</v>
+      </c>
+      <c r="G25" t="n">
+        <v>21.734177625</v>
+      </c>
+      <c r="H25" t="n">
+        <v>3202.85095215</v>
+      </c>
+      <c r="I25" t="n">
+        <v>25.2749745</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>JOÃO PAULO ROSA MART</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>14</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2840.500215</v>
+      </c>
+      <c r="E26" t="n">
+        <v>25.94745</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2944.8930234375</v>
+      </c>
+      <c r="G26" t="n">
+        <v>27.667265625</v>
+      </c>
+      <c r="H26" t="n">
+        <v>3317.0598984375</v>
+      </c>
+      <c r="I26" t="n">
+        <v>33.798515625</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>MATHEUS RODRIGUES DO</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>14</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2685.0158538375</v>
+      </c>
+      <c r="E27" t="n">
+        <v>35.625137625</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2856.80064</v>
+      </c>
+      <c r="G27" t="n">
+        <v>38.4552</v>
+      </c>
+      <c r="H27" t="n">
+        <v>3061.1649144</v>
+      </c>
+      <c r="I27" t="n">
+        <v>41.821992</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CAIO DE ARAÚJO SANTA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>13</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1976.2964694</v>
+      </c>
+      <c r="E28" t="n">
+        <v>28.725642</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2049.09231015</v>
+      </c>
+      <c r="G28" t="n">
+        <v>29.9249145</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2443.5073209375</v>
+      </c>
+      <c r="I28" t="n">
+        <v>36.422690625</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">YAN EMANUEL PEREIRA </t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>13</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2118.07503375</v>
+      </c>
+      <c r="E29" t="n">
+        <v>20.6132625</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2148.7788009375</v>
+      </c>
+      <c r="G29" t="n">
+        <v>21.119090625</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2275.3155384375</v>
+      </c>
+      <c r="I29" t="n">
+        <v>23.203715625</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ISIS CAMPOS SILVA</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>14</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1750.69014</v>
+      </c>
+      <c r="E30" t="n">
+        <v>23.7402</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1946.9039598375</v>
+      </c>
+      <c r="G30" t="n">
+        <v>26.972717625</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2046.1087620375</v>
+      </c>
+      <c r="I30" t="n">
+        <v>28.607063625</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>KAMILY IVENI FERREIR</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>13</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1473.02310375</v>
+      </c>
+      <c r="E31" t="n">
+        <v>22.6733625</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1706.1856509375</v>
+      </c>
+      <c r="G31" t="n">
+        <v>26.514590625</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1876.6083063375</v>
+      </c>
+      <c r="I31" t="n">
+        <v>29.322212625</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>EVELLYN CAROLINY ZAN</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>12</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1230.5716374</v>
+      </c>
+      <c r="E32" t="n">
+        <v>27.783882</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1195.3274343375</v>
+      </c>
+      <c r="G32" t="n">
+        <v>27.203252625</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1495.3162656</v>
+      </c>
+      <c r="I32" t="n">
+        <v>32.145408</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BRUNA MARIA MEDEIROS</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>14</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2156.0548323375</v>
+      </c>
+      <c r="E33" t="n">
+        <v>33.030392625</v>
+      </c>
+      <c r="F33" t="n">
+        <v>2125.2691884375</v>
+      </c>
+      <c r="G33" t="n">
+        <v>32.523215625</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2612.0634609375</v>
+      </c>
+      <c r="I33" t="n">
+        <v>40.542890625</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>NÁTHALY GOTARDI VANS</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>14</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2348.4639045375</v>
+      </c>
+      <c r="E34" t="n">
+        <v>22.990838625</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2473.6236246</v>
+      </c>
+      <c r="G34" t="n">
+        <v>25.052778</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2858.68236015</v>
+      </c>
+      <c r="I34" t="n">
+        <v>31.3964145</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>SOPHIA BRUMATI HELEN</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>11</v>
+      </c>
+      <c r="D35" t="n">
+        <v>724.2111390375002</v>
+      </c>
+      <c r="E35" t="n">
+        <v>16.158173625</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1019.16827415</v>
+      </c>
+      <c r="G35" t="n">
+        <v>21.0174345</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1472.67594135</v>
+      </c>
+      <c r="I35" t="n">
+        <v>28.4887305</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>KARINA DOS SANTOS GO</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>13</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1221.1661133375</v>
+      </c>
+      <c r="E36" t="n">
+        <v>19.718222625</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1356.0989355375</v>
+      </c>
+      <c r="G36" t="n">
+        <v>21.941168625</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1511.5158225375</v>
+      </c>
+      <c r="I36" t="n">
+        <v>24.501578625</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>TAINÁ DA SILVA MOREI</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>12</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1365.87006135</v>
+      </c>
+      <c r="E37" t="n">
+        <v>12.4003305</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1493.9847864</v>
+      </c>
+      <c r="G37" t="n">
+        <v>14.510952</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1798.1567733375</v>
+      </c>
+      <c r="I37" t="n">
+        <v>19.522022625</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MARIA SOFIA BARBOSA </t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>13</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2485.4092824</v>
+      </c>
+      <c r="E38" t="n">
+        <v>17.336232</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2496.63383535</v>
+      </c>
+      <c r="G38" t="n">
+        <v>17.5211505</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2777.5528359375</v>
+      </c>
+      <c r="I38" t="n">
+        <v>22.149140625</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GEOVANI OLIVEIRA DA </t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>13</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1062.6718173375</v>
+      </c>
+      <c r="E39" t="n">
+        <v>22.778942625</v>
+      </c>
+      <c r="F39" t="n">
+        <v>986.7497748374998</v>
+      </c>
+      <c r="G39" t="n">
+        <v>21.528167625</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1331.2274343375</v>
+      </c>
+      <c r="I39" t="n">
+        <v>27.203252625</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KAIQUE GUIMARÃES DE </t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>13</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2450.5637709375</v>
+      </c>
+      <c r="E40" t="n">
+        <v>30.046190625</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2502.51082335</v>
+      </c>
+      <c r="G40" t="n">
+        <v>30.9019905</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2902.9995975375</v>
+      </c>
+      <c r="I40" t="n">
         <v>37.499828625</v>
       </c>
-      <c r="F5" t="n">
-        <v>3180.4332018375</v>
-      </c>
-      <c r="G5" t="n">
-        <v>39.980777625</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3283.5085395375</v>
-      </c>
-      <c r="I5" t="n">
-        <v>41.678888625</v>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>YANG YU OLIVEIRA ALC</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>12</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1476.6504555375</v>
+      </c>
+      <c r="E41" t="n">
+        <v>27.434768625</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1504.9351380375</v>
+      </c>
+      <c r="G41" t="n">
+        <v>27.900743625</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1754.9717313375</v>
+      </c>
+      <c r="I41" t="n">
+        <v>32.019962625</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MARCOS ANTONIO MAHL </t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>13</v>
+      </c>
+      <c r="D42" t="n">
+        <v>2777.5176096</v>
+      </c>
+      <c r="E42" t="n">
+        <v>24.611328</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2811.0498450375</v>
+      </c>
+      <c r="G42" t="n">
+        <v>25.163753625</v>
+      </c>
+      <c r="H42" t="n">
+        <v>3137.0084808375</v>
+      </c>
+      <c r="I42" t="n">
+        <v>30.533747625</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>PAULO VITOR FERREIRA</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>14</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1361.9416374</v>
+      </c>
+      <c r="E43" t="n">
+        <v>27.783882</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1611.47208375</v>
+      </c>
+      <c r="G43" t="n">
+        <v>31.8947625</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1993.04733735</v>
+      </c>
+      <c r="I43" t="n">
+        <v>38.1810105</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>LOGAN REIS HELENO AL</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>14</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2306.02236015</v>
+      </c>
+      <c r="E44" t="n">
+        <v>31.3964145</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2412.93846</v>
+      </c>
+      <c r="G44" t="n">
+        <v>33.1578</v>
+      </c>
+      <c r="H44" t="n">
+        <v>2701.2635814</v>
+      </c>
+      <c r="I44" t="n">
+        <v>37.907802</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>RAICK ARTHUR DOS SAN</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>12</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3147.2639136</v>
+      </c>
+      <c r="E45" t="n">
+        <v>45.330048</v>
+      </c>
+      <c r="F45" t="n">
+        <v>3220.1490744</v>
+      </c>
+      <c r="G45" t="n">
+        <v>46.530792</v>
+      </c>
+      <c r="H45" t="n">
+        <v>4286.5783680375</v>
+      </c>
+      <c r="I45" t="n">
+        <v>64.099643625</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>RENAN ESCAVASSINI BR</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>14</v>
+      </c>
+      <c r="D46" t="n">
+        <v>4290.8851380375</v>
+      </c>
+      <c r="E46" t="n">
+        <v>27.900743625</v>
+      </c>
+      <c r="F46" t="n">
+        <v>4340.9564694</v>
+      </c>
+      <c r="G46" t="n">
+        <v>28.725642</v>
+      </c>
+      <c r="H46" t="n">
+        <v>4503.07236015</v>
+      </c>
+      <c r="I46" t="n">
+        <v>31.3964145</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ARTHUR EDUARDO DA SI</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>13</v>
+      </c>
+      <c r="D47" t="n">
+        <v>3468.16232415</v>
+      </c>
+      <c r="E47" t="n">
+        <v>42.1089345</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3476.8933590375</v>
+      </c>
+      <c r="G47" t="n">
+        <v>42.252773625</v>
+      </c>
+      <c r="H47" t="n">
+        <v>3913.4897634375</v>
+      </c>
+      <c r="I47" t="n">
+        <v>49.445465625</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CAIO CHRISTIAN ARTIG</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>14</v>
+      </c>
+      <c r="D48" t="n">
+        <v>2829.5115264</v>
+      </c>
+      <c r="E48" t="n">
+        <v>36.289152</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2757.2292759375</v>
+      </c>
+      <c r="G48" t="n">
+        <v>35.098340625</v>
+      </c>
+      <c r="H48" t="n">
+        <v>3324.25528335</v>
+      </c>
+      <c r="I48" t="n">
+        <v>44.4397905</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>JUNIOR DOS SANTOS RE</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>14</v>
+      </c>
+      <c r="D49" t="n">
+        <v>2339.8318374</v>
+      </c>
+      <c r="E49" t="n">
+        <v>33.669882</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2379.0210093375</v>
+      </c>
+      <c r="G49" t="n">
+        <v>34.315502625</v>
+      </c>
+      <c r="H49" t="n">
+        <v>2904.6918336</v>
+      </c>
+      <c r="I49" t="n">
+        <v>42.975648</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>DAVI HUDSON CARMARGO</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>14</v>
+      </c>
+      <c r="D50" t="n">
+        <v>3692.9118336</v>
+      </c>
+      <c r="E50" t="n">
+        <v>42.975648</v>
+      </c>
+      <c r="F50" t="n">
+        <v>3835.8239136</v>
+      </c>
+      <c r="G50" t="n">
+        <v>45.330048</v>
+      </c>
+      <c r="H50" t="n">
+        <v>4180.9044834375</v>
+      </c>
+      <c r="I50" t="n">
+        <v>51.015065625</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>PEDRO HENRIQUE FRANÇ</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>14</v>
+      </c>
+      <c r="D51" t="n">
+        <v>2305.68827415</v>
+      </c>
+      <c r="E51" t="n">
+        <v>21.0174345</v>
+      </c>
+      <c r="F51" t="n">
+        <v>2156.2632738375</v>
+      </c>
+      <c r="G51" t="n">
+        <v>18.555737625</v>
+      </c>
+      <c r="H51" t="n">
+        <v>2374.3828359375</v>
+      </c>
+      <c r="I51" t="n">
+        <v>22.149140625</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>RENAN ALVES PAZETO</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>13</v>
+      </c>
+      <c r="D52" t="n">
+        <v>3014.26959375</v>
+      </c>
+      <c r="E52" t="n">
+        <v>37.0940625</v>
+      </c>
+      <c r="F52" t="n">
+        <v>3121.9672440375</v>
+      </c>
+      <c r="G52" t="n">
+        <v>38.868323625</v>
+      </c>
+      <c r="H52" t="n">
+        <v>3577.9163259375</v>
+      </c>
+      <c r="I52" t="n">
+        <v>46.379840625</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>GABRIEL TEIXEIRA AMA</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>14</v>
+      </c>
+      <c r="D53" t="n">
+        <v>2772.8040486</v>
+      </c>
+      <c r="E53" t="n">
+        <v>29.683098</v>
+      </c>
+      <c r="F53" t="n">
+        <v>2983.71846</v>
+      </c>
+      <c r="G53" t="n">
+        <v>33.1578</v>
+      </c>
+      <c r="H53" t="n">
+        <v>3588.4821885375</v>
+      </c>
+      <c r="I53" t="n">
+        <v>43.120958625</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>LUIZ EDUARDO TURATTO</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>13</v>
+      </c>
+      <c r="D54" t="n">
+        <v>2334.6957345375</v>
+      </c>
+      <c r="E54" t="n">
+        <v>17.987738625</v>
+      </c>
+      <c r="F54" t="n">
+        <v>2295.1492824</v>
+      </c>
+      <c r="G54" t="n">
+        <v>17.336232</v>
+      </c>
+      <c r="H54" t="n">
+        <v>2512.4426340375</v>
+      </c>
+      <c r="I54" t="n">
+        <v>20.916023625</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KAIO MURILLO ARAÚJO </t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>13</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1947.81827415</v>
+      </c>
+      <c r="E55" t="n">
+        <v>21.0174345</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2054.7418173375</v>
+      </c>
+      <c r="G55" t="n">
+        <v>22.778942625</v>
+      </c>
+      <c r="H55" t="n">
+        <v>2247.070215</v>
+      </c>
+      <c r="I55" t="n">
+        <v>25.94745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>